<commit_message>
Update Años Texto Proyecciones.xlsx
</commit_message>
<xml_diff>
--- a/Proyecciones de Población/Años Texto Proyecciones.xlsx
+++ b/Proyecciones de Población/Años Texto Proyecciones.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-MUNI\Proyecciones de Población\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86F57404-1E37-41E8-BC75-3AA28FDB4F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3613180B-F0F5-40EF-A691-D61A7F4931BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5F128AE3-A9E6-4842-9602-467FBC885F26}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{5F128AE3-A9E6-4842-9602-467FBC885F26}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Categoría Edad" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Año Texto</t>
   </si>
@@ -140,6 +141,90 @@
   </si>
   <si>
     <t>2035</t>
+  </si>
+  <si>
+    <t>Rango Edad</t>
+  </si>
+  <si>
+    <t>01. 0 a 5 años</t>
+  </si>
+  <si>
+    <t>02. 6 a 10 años</t>
+  </si>
+  <si>
+    <t>03. 11 a 15 años</t>
+  </si>
+  <si>
+    <t>04. 16 a 20 años</t>
+  </si>
+  <si>
+    <t>05. 21 a 25 años</t>
+  </si>
+  <si>
+    <t>06. 26 a 30 años</t>
+  </si>
+  <si>
+    <t>07. 31 a 35 años</t>
+  </si>
+  <si>
+    <t>08. 36 a 40 años</t>
+  </si>
+  <si>
+    <t>09. 41 a 45 años</t>
+  </si>
+  <si>
+    <t>10. 46 a 50 años</t>
+  </si>
+  <si>
+    <t>11. 51 a 55 años</t>
+  </si>
+  <si>
+    <t>12. 56 a 60 años</t>
+  </si>
+  <si>
+    <t>13. 61 a 65 años</t>
+  </si>
+  <si>
+    <t>14. 66 a 70 años</t>
+  </si>
+  <si>
+    <t>15. 71 a 75 años</t>
+  </si>
+  <si>
+    <t>16. 76 a 80 años</t>
+  </si>
+  <si>
+    <t>17. más de 80 años</t>
+  </si>
+  <si>
+    <t>Categoría 1</t>
+  </si>
+  <si>
+    <t>Categoría 2</t>
+  </si>
+  <si>
+    <t>Estudiantes (6 a 25 años)</t>
+  </si>
+  <si>
+    <t>Trabajadores (26 a 65 años)</t>
+  </si>
+  <si>
+    <t>3era Edad (65 y más años)</t>
+  </si>
+  <si>
+    <t>Primera Infancia (0 a 5 años)</t>
+  </si>
+  <si>
+    <t>4ta Edad (76 y más años)</t>
+  </si>
+  <si>
+    <t>3era Edad (65 a 75 años)</t>
+  </si>
+  <si>
+    <t>Educación Básica-Media (6 a 20 años)</t>
+  </si>
+  <si>
+    <t>Educación Universitaria (21-25 años)</t>
   </si>
 </sst>
 </file>
@@ -500,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57F9458-AC4E-4B52-8A6D-FBED3F5AF474}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,4 +867,220 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7370D3-5C66-47B5-9BA2-C442B2BA677B}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>